<commit_message>
Return "" for null date columns, trim empty trailing rows
</commit_message>
<xml_diff>
--- a/pandas/tests/io/data/excel/dimension_large.xlsx
+++ b/pandas/tests/io/data/excel/dimension_large.xlsx
@@ -173,7 +173,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -230,6 +230,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="16">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Removed fix for 39181
</commit_message>
<xml_diff>
--- a/pandas/tests/io/data/excel/dimension_large.xlsx
+++ b/pandas/tests/io/data/excel/dimension_large.xlsx
@@ -230,14 +230,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>